<commit_message>
Added letter excel files for labelling
</commit_message>
<xml_diff>
--- a/results/comparison-letters-templates/lmb_comparison_letters_within_season.xlsx
+++ b/results/comparison-letters-templates/lmb_comparison_letters_within_season.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\comparison-letters-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3C0A5-7D96-4F90-9F0B-CA4C49D0463A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430AA4D0-262D-4B3E-A9C6-B9C37193DED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A924BF9-6E79-484A-812B-34246742B6BC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9A924BF9-6E79-484A-812B-34246742B6BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="24">
   <si>
     <t xml:space="preserve">Habitat Type </t>
   </si>
@@ -101,19 +101,13 @@
     <t>e</t>
   </si>
   <si>
-    <t>de</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
     <t>g</t>
   </si>
   <si>
-    <t>gh</t>
-  </si>
-  <si>
-    <t>gi</t>
+    <t>fg</t>
   </si>
 </sst>
 </file>
@@ -179,25 +173,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958CDEBC-A36B-40FB-93F3-09AA5706FC28}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,51 +593,51 @@
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>18</v>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -657,19 +645,19 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -677,19 +665,19 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -697,19 +685,19 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -762,15 +750,15 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H14" t="s">
@@ -783,10 +771,10 @@
         <v>15</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -833,15 +821,15 @@
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -894,54 +882,54 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>22</v>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -949,19 +937,19 @@
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -969,19 +957,19 @@
       <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -989,19 +977,19 @@
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="7" t="s">
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1054,54 +1042,54 @@
       <c r="A34" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="6" t="s">
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="H34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="I34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="J34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>25</v>
+      <c r="L34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="B35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1109,19 +1097,19 @@
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="6" t="s">
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1129,19 +1117,19 @@
       <c r="A37" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1149,19 +1137,19 @@
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="7" t="s">
+      <c r="B38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>